<commit_message>
Final checkin before Durandal integration
</commit_message>
<xml_diff>
--- a/_SolutionItems/ToDo.xlsx
+++ b/_SolutionItems/ToDo.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="259">
   <si>
     <t>Type</t>
   </si>
@@ -816,6 +816,15 @@
   </si>
   <si>
     <t>Revolution Slider already done. Need to do the same for FlexSlider, View360 and others.</t>
+  </si>
+  <si>
+    <t>UPDATE: They are working fine. We just need to remember to enable the ones we want. Also, we must restart the app when making changes (enable/disable or change interval, etc)</t>
+  </si>
+  <si>
+    <t>Make "Create Sample Data" option work.</t>
+  </si>
+  <si>
+    <t>Set Kore theme as the default when installing a new system.</t>
   </si>
 </sst>
 </file>
@@ -1293,8 +1302,8 @@
   <dimension ref="A1:H229"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A136" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G146" sqref="G146"/>
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E151" sqref="E151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2532,7 +2541,7 @@
       <c r="G58" s="14"/>
       <c r="H58" s="14"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="6">
         <v>58</v>
       </c>
@@ -2550,27 +2559,27 @@
       <c r="G59" s="14"/>
       <c r="H59" s="14"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A60" s="6">
+    <row r="60" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="9">
         <v>59</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B60" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C60" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D60" s="6"/>
-      <c r="E60" s="13" t="s">
+      <c r="C60" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D60" s="9"/>
+      <c r="E60" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="F60" s="13" t="s">
+      <c r="F60" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G60" s="21"/>
+      <c r="H60" s="21"/>
+    </row>
+    <row r="61" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A61" s="6">
         <v>60</v>
       </c>
@@ -3526,23 +3535,27 @@
         <v>42188</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A107" s="8">
+    <row r="107" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A107" s="10">
         <v>106</v>
       </c>
-      <c r="B107" s="8" t="s">
+      <c r="B107" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C107" s="8" t="s">
+      <c r="C107" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D107" s="8"/>
-      <c r="E107" s="17" t="s">
+      <c r="D107" s="10"/>
+      <c r="E107" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="F107" s="17"/>
-      <c r="G107" s="18"/>
-      <c r="H107" s="18"/>
+      <c r="F107" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="G107" s="12"/>
+      <c r="H107" s="12">
+        <v>42214</v>
+      </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A108" s="10">
@@ -4431,28 +4444,48 @@
       <c r="H146" s="24"/>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A147" s="2">
+      <c r="A147" s="7">
         <v>146</v>
       </c>
-      <c r="B147" s="2"/>
-      <c r="C147" s="2"/>
-      <c r="D147" s="2"/>
-      <c r="E147" s="4"/>
-      <c r="F147" s="4"/>
-      <c r="G147" s="3"/>
-      <c r="H147" s="3"/>
+      <c r="B147" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C147" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D147" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E147" s="15" t="s">
+        <v>257</v>
+      </c>
+      <c r="F147" s="15"/>
+      <c r="G147" s="16">
+        <v>42214</v>
+      </c>
+      <c r="H147" s="16"/>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A148" s="2">
+      <c r="A148" s="7">
         <v>147</v>
       </c>
-      <c r="B148" s="2"/>
-      <c r="C148" s="2"/>
-      <c r="D148" s="2"/>
-      <c r="E148" s="4"/>
-      <c r="F148" s="4"/>
-      <c r="G148" s="3"/>
-      <c r="H148" s="3"/>
+      <c r="B148" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C148" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D148" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E148" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="F148" s="15"/>
+      <c r="G148" s="16">
+        <v>42214</v>
+      </c>
+      <c r="H148" s="16"/>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A149" s="2">

</xml_diff>

<commit_message>
Update to OData v5.7 to solve this issue: https://github.com/OData/WebApi/issues/484#issuecomment-153929767
</commit_message>
<xml_diff>
--- a/_SolutionItems/ToDo.xlsx
+++ b/_SolutionItems/ToDo.xlsx
@@ -15,6 +15,9 @@
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
     <sheet name="Legend" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="268">
   <si>
     <t>Type</t>
   </si>
@@ -841,12 +844,24 @@
   <si>
     <t>So we can show different content based on group (example: US customers vs UK customers, etc)</t>
   </si>
+  <si>
+    <t>Pages: Use something like a drilldown menu in place of the page dropdowns</t>
+  </si>
+  <si>
+    <t>Copy from nopCommerce and just need to modify the UI</t>
+  </si>
+  <si>
+    <t>TinyMCE: images dont have leading slash</t>
+  </si>
+  <si>
+    <t>TinyMCE doesn't add a leading slash and so if the current page url is not the root, then the images don't display</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -895,6 +910,12 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1045,7 +1066,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1097,6 +1118,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1106,8 +1132,36 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1385,8 +1439,8 @@
   <dimension ref="A1:H229"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H145" sqref="H145"/>
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E151" sqref="E151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2119,24 +2173,26 @@
       <c r="H33" s="14"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="7">
+      <c r="A34" s="10">
         <v>33</v>
       </c>
-      <c r="B34" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" s="7" t="s">
+      <c r="B34" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F34" s="15"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12">
+        <v>42275</v>
+      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
@@ -3358,7 +3414,7 @@
       <c r="G93" s="14"/>
       <c r="H93" s="14"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A94" s="6">
         <v>93</v>
       </c>
@@ -3374,29 +3430,31 @@
       <c r="E94" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="F94" s="13"/>
+      <c r="F94" s="13" t="s">
+        <v>265</v>
+      </c>
       <c r="G94" s="14"/>
       <c r="H94" s="14"/>
     </row>
-    <row r="95" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="6">
+    <row r="95" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="9">
         <v>94</v>
       </c>
-      <c r="B95" s="6" t="s">
+      <c r="B95" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C95" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D95" s="6" t="s">
+      <c r="C95" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D95" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E95" s="13" t="s">
+      <c r="E95" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="F95" s="13"/>
-      <c r="G95" s="14"/>
-      <c r="H95" s="14"/>
+      <c r="F95" s="20"/>
+      <c r="G95" s="21"/>
+      <c r="H95" s="21"/>
     </row>
     <row r="96" spans="1:8" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96" s="9">
@@ -4133,28 +4191,28 @@
       <c r="H128" s="24"/>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A129" s="22">
+      <c r="A129" s="10">
         <v>128</v>
       </c>
-      <c r="B129" s="22" t="s">
+      <c r="B129" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C129" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D129" s="22" t="s">
+      <c r="C129" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D129" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="E129" s="23" t="s">
+      <c r="E129" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="F129" s="23" t="s">
+      <c r="F129" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="G129" s="24">
+      <c r="G129" s="12">
         <v>42192</v>
       </c>
-      <c r="H129" s="24"/>
+      <c r="H129" s="12"/>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130" s="22">
@@ -4347,26 +4405,26 @@
       <c r="H137" s="24"/>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A138" s="10">
+      <c r="A138" s="33">
         <v>137</v>
       </c>
-      <c r="B138" s="10" t="s">
+      <c r="B138" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C138" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D138" s="10" t="s">
+      <c r="C138" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D138" s="33" t="s">
         <v>121</v>
       </c>
-      <c r="E138" s="11" t="s">
+      <c r="E138" s="34" t="s">
         <v>235</v>
       </c>
-      <c r="F138" s="11"/>
-      <c r="G138" s="12">
+      <c r="F138" s="34"/>
+      <c r="G138" s="35">
         <v>42194</v>
       </c>
-      <c r="H138" s="12"/>
+      <c r="H138" s="35"/>
     </row>
     <row r="139" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A139" s="22">
@@ -4590,29 +4648,49 @@
       </c>
       <c r="H148" s="16"/>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A149" s="2">
+    <row r="149" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A149" s="22">
         <v>148</v>
       </c>
-      <c r="B149" s="2"/>
-      <c r="C149" s="2"/>
-      <c r="D149" s="2"/>
-      <c r="E149" s="4"/>
-      <c r="F149" s="4"/>
-      <c r="G149" s="3"/>
-      <c r="H149" s="3"/>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A150" s="2">
+      <c r="B149" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C149" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D149" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="E149" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="F149" s="23"/>
+      <c r="G149" s="24">
+        <v>42317</v>
+      </c>
+      <c r="H149" s="24"/>
+    </row>
+    <row r="150" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A150" s="7">
         <v>149</v>
       </c>
-      <c r="B150" s="2"/>
-      <c r="C150" s="2"/>
-      <c r="D150" s="2"/>
-      <c r="E150" s="4"/>
-      <c r="F150" s="4"/>
-      <c r="G150" s="3"/>
-      <c r="H150" s="3"/>
+      <c r="B150" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C150" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D150" s="7"/>
+      <c r="E150" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="F150" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="G150" s="16">
+        <v>42317</v>
+      </c>
+      <c r="H150" s="16"/>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151" s="2">

</xml_diff>

<commit_message>
Language Switch in default setup if "Create Sample Data" is checked.
</commit_message>
<xml_diff>
--- a/_SolutionItems/ToDo.xlsx
+++ b/_SolutionItems/ToDo.xlsx
@@ -860,7 +860,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1439,8 +1439,8 @@
   <dimension ref="A1:H229"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E151" sqref="E151"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1593,26 +1593,28 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
+      <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="6" t="s">
+      <c r="C7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12">
+        <v>42345</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
@@ -1675,26 +1677,28 @@
       <c r="H10" s="14"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
+      <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="6" t="s">
+      <c r="B11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F11" s="11"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12">
+        <v>42345</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -1716,25 +1720,25 @@
         <v>42207</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="6">
-        <v>12</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="13" t="s">
+    <row r="13" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="9">
+        <v>12</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F13" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
     </row>
     <row r="14" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9">

</xml_diff>

<commit_message>
Started work on forums plugin
</commit_message>
<xml_diff>
--- a/_SolutionItems/ToDo.xlsx
+++ b/_SolutionItems/ToDo.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="269">
   <si>
     <t>Type</t>
   </si>
@@ -802,59 +802,63 @@
     <t>Ecommerce: Allow user to specify city if none are set for selected country</t>
   </si>
   <si>
+    <t>UPDATE: This should be able to be fixed when #143 is done (Durandal)</t>
+  </si>
+  <si>
+    <t>Use proper HTML5 semantic tags everywhere</t>
+  </si>
+  <si>
+    <t>Localization: Show TextArea instead of TextBox when editing localizable strings.</t>
+  </si>
+  <si>
+    <t>Add help text for complex blocks</t>
+  </si>
+  <si>
+    <t>Revolution Slider already done. Need to do the same for FlexSlider, View360 and others.</t>
+  </si>
+  <si>
+    <t>UPDATE: They are working fine. We just need to remember to enable the ones we want. Also, we must restart the app when making changes (enable/disable or change interval, etc)</t>
+  </si>
+  <si>
+    <t>Make "Create Sample Data" option work.</t>
+  </si>
+  <si>
+    <t>Set Kore theme as the default when installing a new system.</t>
+  </si>
+  <si>
+    <t>No longer necessary since we moved to Odata v4, so we no longer have that limitation of only 3 levels</t>
+  </si>
+  <si>
+    <t>No Longer Needed</t>
+  </si>
+  <si>
+    <t>Added output caching and we can turn it on/off in web.config</t>
+  </si>
+  <si>
+    <t>MVC6 seems to have support for this built-in… so we wait for that instead</t>
+  </si>
+  <si>
+    <t>So we can show different content based on group (example: US customers vs UK customers, etc)</t>
+  </si>
+  <si>
+    <t>Pages: Use something like a drilldown menu in place of the page dropdowns</t>
+  </si>
+  <si>
+    <t>Copy from nopCommerce and just need to modify the UI</t>
+  </si>
+  <si>
+    <t>TinyMCE: images dont have leading slash</t>
+  </si>
+  <si>
+    <t>TinyMCE doesn't add a leading slash and so if the current page url is not the root, then the images don't display</t>
+  </si>
+  <si>
+    <t>2015-12-15: Started working on this already last week: the language switch is created by default when "Create Sample Data" is selected. Will add more over time.</t>
+  </si>
+  <si>
     <t>Example: TinyMCE should not be included by default and should be loaded from specific blocks that need it.. This will also affect other libs (not only TinyMCE)..!
-UPDATE: This should be able to be fixed when #143 is done (Durandal)</t>
-  </si>
-  <si>
-    <t>UPDATE: This should be able to be fixed when #143 is done (Durandal)</t>
-  </si>
-  <si>
-    <t>Use proper HTML5 semantic tags everywhere</t>
-  </si>
-  <si>
-    <t>Localization: Show TextArea instead of TextBox when editing localizable strings.</t>
-  </si>
-  <si>
-    <t>Add help text for complex blocks</t>
-  </si>
-  <si>
-    <t>Revolution Slider already done. Need to do the same for FlexSlider, View360 and others.</t>
-  </si>
-  <si>
-    <t>UPDATE: They are working fine. We just need to remember to enable the ones we want. Also, we must restart the app when making changes (enable/disable or change interval, etc)</t>
-  </si>
-  <si>
-    <t>Make "Create Sample Data" option work.</t>
-  </si>
-  <si>
-    <t>Set Kore theme as the default when installing a new system.</t>
-  </si>
-  <si>
-    <t>No longer necessary since we moved to Odata v4, so we no longer have that limitation of only 3 levels</t>
-  </si>
-  <si>
-    <t>No Longer Needed</t>
-  </si>
-  <si>
-    <t>Added output caching and we can turn it on/off in web.config</t>
-  </si>
-  <si>
-    <t>MVC6 seems to have support for this built-in… so we wait for that instead</t>
-  </si>
-  <si>
-    <t>So we can show different content based on group (example: US customers vs UK customers, etc)</t>
-  </si>
-  <si>
-    <t>Pages: Use something like a drilldown menu in place of the page dropdowns</t>
-  </si>
-  <si>
-    <t>Copy from nopCommerce and just need to modify the UI</t>
-  </si>
-  <si>
-    <t>TinyMCE: images dont have leading slash</t>
-  </si>
-  <si>
-    <t>TinyMCE doesn't add a leading slash and so if the current page url is not the root, then the images don't display</t>
+UPDATE: This should be able to be fixed when #143 is done (Durandal)
+2015-12-15: Durandal was implemented months ago. Need to look at this again ASAP.</t>
   </si>
 </sst>
 </file>
@@ -1439,8 +1443,8 @@
   <dimension ref="A1:H229"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1541,7 +1545,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="26" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G4" s="27"/>
       <c r="H4" s="27">
@@ -2112,7 +2116,7 @@
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
     </row>
-    <row r="31" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" s="8">
         <v>30</v>
       </c>
@@ -2129,7 +2133,7 @@
         <v>70</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>250</v>
+        <v>268</v>
       </c>
       <c r="G31" s="18"/>
       <c r="H31" s="18"/>
@@ -2401,7 +2405,7 @@
         <v>85</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G44" s="14"/>
       <c r="H44" s="14"/>
@@ -3101,7 +3105,7 @@
         <v>143</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G78" s="12"/>
       <c r="H78" s="12">
@@ -3120,7 +3124,7 @@
       </c>
       <c r="D79" s="9"/>
       <c r="E79" s="20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F79" s="20"/>
       <c r="G79" s="21"/>
@@ -3391,7 +3395,7 @@
         <v>165</v>
       </c>
       <c r="F92" s="20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G92" s="21"/>
       <c r="H92" s="21"/>
@@ -3435,7 +3439,7 @@
         <v>167</v>
       </c>
       <c r="F94" s="13" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G94" s="14"/>
       <c r="H94" s="14"/>
@@ -3477,7 +3481,7 @@
         <v>169</v>
       </c>
       <c r="F96" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G96" s="21"/>
       <c r="H96" s="21"/>
@@ -3713,7 +3717,7 @@
         <v>187</v>
       </c>
       <c r="F107" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G107" s="12"/>
       <c r="H107" s="12">
@@ -4576,7 +4580,7 @@
         <v>94</v>
       </c>
       <c r="E145" s="23" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F145" s="23"/>
       <c r="G145" s="24">
@@ -4598,37 +4602,41 @@
         <v>94</v>
       </c>
       <c r="E146" s="23" t="s">
+        <v>253</v>
+      </c>
+      <c r="F146" s="23" t="s">
         <v>254</v>
-      </c>
-      <c r="F146" s="23" t="s">
-        <v>255</v>
       </c>
       <c r="G146" s="24">
         <v>42214</v>
       </c>
       <c r="H146" s="24"/>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A147" s="7">
+    <row r="147" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A147" s="10">
         <v>146</v>
       </c>
-      <c r="B147" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C147" s="7" t="s">
+      <c r="B147" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C147" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D147" s="7" t="s">
+      <c r="D147" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E147" s="15" t="s">
-        <v>257</v>
-      </c>
-      <c r="F147" s="15"/>
-      <c r="G147" s="16">
+      <c r="E147" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="F147" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="G147" s="12">
         <v>42214</v>
       </c>
-      <c r="H147" s="16"/>
+      <c r="H147" s="12">
+        <v>42353</v>
+      </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A148" s="7">
@@ -4644,7 +4652,7 @@
         <v>25</v>
       </c>
       <c r="E148" s="15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F148" s="15"/>
       <c r="G148" s="16">
@@ -4666,7 +4674,7 @@
         <v>94</v>
       </c>
       <c r="E149" s="23" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F149" s="23"/>
       <c r="G149" s="24">
@@ -4675,26 +4683,26 @@
       <c r="H149" s="24"/>
     </row>
     <row r="150" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A150" s="7">
+      <c r="A150" s="8">
         <v>149</v>
       </c>
-      <c r="B150" s="7" t="s">
+      <c r="B150" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C150" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D150" s="7"/>
-      <c r="E150" s="15" t="s">
+      <c r="C150" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D150" s="8"/>
+      <c r="E150" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="F150" s="17" t="s">
         <v>266</v>
       </c>
-      <c r="F150" s="15" t="s">
-        <v>267</v>
-      </c>
-      <c r="G150" s="16">
+      <c r="G150" s="18">
         <v>42317</v>
       </c>
-      <c r="H150" s="16"/>
+      <c r="H150" s="18"/>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A151" s="2">
@@ -5582,7 +5590,7 @@
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="25"/>
       <c r="B6" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finally solved the razor intellisense issues in plugins!
</commit_message>
<xml_diff>
--- a/_SolutionItems/ToDo.xlsx
+++ b/_SolutionItems/ToDo.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="273">
   <si>
     <t>Type</t>
   </si>
@@ -511,9 +511,6 @@
     <t>Razor intellisense not working for class libraries</t>
   </si>
   <si>
-    <t>Might be a bug with Visual Studio</t>
-  </si>
-  <si>
     <t>On Page Editing</t>
   </si>
   <si>
@@ -868,6 +865,12 @@
   </si>
   <si>
     <t>Ignore this. Multiple routes are better</t>
+  </si>
+  <si>
+    <t>MVC6 seems to have some new localization mechanism. Needs investigation.</t>
+  </si>
+  <si>
+    <t>Finally solved it! Was indeed a Visual Studio issue. Nop has the same problem.</t>
   </si>
 </sst>
 </file>
@@ -1452,8 +1455,8 @@
   <dimension ref="A1:H229"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F141" sqref="F141"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1554,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="26" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G4" s="27"/>
       <c r="H4" s="27">
@@ -1741,7 +1744,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="20" t="s">
@@ -1761,7 +1764,7 @@
         <v>31</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>32</v>
@@ -2142,7 +2145,7 @@
         <v>70</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G31" s="18"/>
       <c r="H31" s="18"/>
@@ -2369,7 +2372,7 @@
         <v>55</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F42" s="13"/>
       <c r="G42" s="14"/>
@@ -2389,7 +2392,7 @@
         <v>55</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F43" s="15" t="s">
         <v>84</v>
@@ -2414,7 +2417,7 @@
         <v>85</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G44" s="14"/>
       <c r="H44" s="14"/>
@@ -2447,7 +2450,7 @@
         <v>31</v>
       </c>
       <c r="C46" s="30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D46" s="30" t="s">
         <v>86</v>
@@ -2469,7 +2472,7 @@
         <v>91</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D47" s="9" t="s">
         <v>86</v>
@@ -2489,7 +2492,7 @@
         <v>12</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D48" s="9"/>
       <c r="E48" s="20" t="s">
@@ -2731,7 +2734,7 @@
         <v>31</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D60" s="9"/>
       <c r="E60" s="20" t="s">
@@ -3116,7 +3119,7 @@
         <v>143</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G78" s="12"/>
       <c r="H78" s="12">
@@ -3131,11 +3134,11 @@
         <v>91</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D79" s="9"/>
       <c r="E79" s="20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F79" s="20"/>
       <c r="G79" s="21"/>
@@ -3246,24 +3249,26 @@
       <c r="H84" s="14"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A85" s="7">
+      <c r="A85" s="10">
         <v>84</v>
       </c>
-      <c r="B85" s="7" t="s">
+      <c r="B85" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C85" s="7" t="s">
+      <c r="C85" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D85" s="7"/>
-      <c r="E85" s="15" t="s">
+      <c r="D85" s="10"/>
+      <c r="E85" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="F85" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="G85" s="16"/>
-      <c r="H85" s="16"/>
+      <c r="F85" s="11" t="s">
+        <v>272</v>
+      </c>
+      <c r="G85" s="12"/>
+      <c r="H85" s="12">
+        <v>42402</v>
+      </c>
     </row>
     <row r="86" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="6">
@@ -3279,10 +3284,10 @@
         <v>94</v>
       </c>
       <c r="E86" s="13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F86" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G86" s="14"/>
       <c r="H86" s="14"/>
@@ -3295,14 +3300,14 @@
         <v>91</v>
       </c>
       <c r="C87" s="30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D87" s="30"/>
       <c r="E87" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="F87" s="31" t="s">
         <v>156</v>
-      </c>
-      <c r="F87" s="31" t="s">
-        <v>157</v>
       </c>
       <c r="G87" s="32"/>
       <c r="H87" s="32">
@@ -3317,16 +3322,16 @@
         <v>12</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E88" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="F88" s="20" t="s">
         <v>158</v>
-      </c>
-      <c r="F88" s="20" t="s">
-        <v>159</v>
       </c>
       <c r="G88" s="21"/>
       <c r="H88" s="21"/>
@@ -3339,15 +3344,17 @@
         <v>88</v>
       </c>
       <c r="C89" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D89" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E89" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="F89" s="20"/>
+        <v>159</v>
+      </c>
+      <c r="F89" s="20" t="s">
+        <v>271</v>
+      </c>
       <c r="G89" s="21"/>
       <c r="H89" s="21"/>
     </row>
@@ -3365,15 +3372,15 @@
         <v>86</v>
       </c>
       <c r="E90" s="26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F90" s="26" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G90" s="27"/>
       <c r="H90" s="27"/>
     </row>
-    <row r="91" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91" s="6">
         <v>90</v>
       </c>
@@ -3385,35 +3392,35 @@
       </c>
       <c r="D91" s="6"/>
       <c r="E91" s="13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F91" s="13"/>
       <c r="G91" s="14"/>
       <c r="H91" s="14"/>
     </row>
-    <row r="92" spans="1:8" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="9">
+    <row r="92" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A92" s="25">
         <v>91</v>
       </c>
-      <c r="B92" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C92" s="9" t="s">
+      <c r="B92" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C92" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="D92" s="25" t="s">
+        <v>160</v>
+      </c>
+      <c r="E92" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="D92" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="E92" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="F92" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="G92" s="21"/>
-      <c r="H92" s="21"/>
-    </row>
-    <row r="93" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="F92" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="G92" s="27"/>
+      <c r="H92" s="27"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93" s="6">
         <v>92</v>
       </c>
@@ -3424,13 +3431,13 @@
         <v>8</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E93" s="13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G93" s="14"/>
       <c r="H93" s="14"/>
@@ -3449,10 +3456,10 @@
         <v>55</v>
       </c>
       <c r="E94" s="11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F94" s="11" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G94" s="12"/>
       <c r="H94" s="12">
@@ -3467,13 +3474,13 @@
         <v>31</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D95" s="9" t="s">
         <v>55</v>
       </c>
       <c r="E95" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F95" s="20"/>
       <c r="G95" s="21"/>
@@ -3487,16 +3494,16 @@
         <v>12</v>
       </c>
       <c r="C96" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E96" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F96" s="20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G96" s="21"/>
       <c r="H96" s="21"/>
@@ -3509,16 +3516,16 @@
         <v>31</v>
       </c>
       <c r="C97" s="25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D97" s="25" t="s">
         <v>110</v>
       </c>
       <c r="E97" s="26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F97" s="26" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G97" s="27"/>
       <c r="H97" s="27"/>
@@ -3537,10 +3544,10 @@
         <v>64</v>
       </c>
       <c r="E98" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="F98" s="13" t="s">
         <v>172</v>
-      </c>
-      <c r="F98" s="13" t="s">
-        <v>173</v>
       </c>
       <c r="G98" s="14"/>
       <c r="H98" s="14"/>
@@ -3556,10 +3563,10 @@
         <v>11</v>
       </c>
       <c r="D99" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="E99" s="15" t="s">
         <v>174</v>
-      </c>
-      <c r="E99" s="15" t="s">
-        <v>175</v>
       </c>
       <c r="F99" s="15"/>
       <c r="G99" s="16"/>
@@ -3576,10 +3583,10 @@
         <v>8</v>
       </c>
       <c r="D100" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E100" s="13" t="s">
         <v>176</v>
-      </c>
-      <c r="E100" s="13" t="s">
-        <v>177</v>
       </c>
       <c r="F100" s="13"/>
       <c r="G100" s="14"/>
@@ -3596,13 +3603,13 @@
         <v>8</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E101" s="13" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F101" s="13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G101" s="14"/>
       <c r="H101" s="14"/>
@@ -3618,13 +3625,13 @@
         <v>62</v>
       </c>
       <c r="D102" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E102" s="11" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F102" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G102" s="12"/>
       <c r="H102" s="12">
@@ -3639,16 +3646,16 @@
         <v>144</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D103" s="9" t="s">
         <v>63</v>
       </c>
       <c r="E103" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="F103" s="20" t="s">
         <v>181</v>
-      </c>
-      <c r="F103" s="20" t="s">
-        <v>182</v>
       </c>
       <c r="G103" s="21"/>
       <c r="H103" s="21"/>
@@ -3667,10 +3674,10 @@
         <v>55</v>
       </c>
       <c r="E104" s="13" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F104" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G104" s="14"/>
       <c r="H104" s="14"/>
@@ -3689,10 +3696,10 @@
         <v>94</v>
       </c>
       <c r="E105" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="F105" s="13" t="s">
         <v>184</v>
-      </c>
-      <c r="F105" s="13" t="s">
-        <v>185</v>
       </c>
       <c r="G105" s="14"/>
       <c r="H105" s="14"/>
@@ -3711,7 +3718,7 @@
         <v>55</v>
       </c>
       <c r="E106" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F106" s="11"/>
       <c r="G106" s="12"/>
@@ -3731,10 +3738,10 @@
       </c>
       <c r="D107" s="10"/>
       <c r="E107" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F107" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G107" s="12"/>
       <c r="H107" s="12">
@@ -3755,10 +3762,10 @@
         <v>7</v>
       </c>
       <c r="E108" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="F108" s="11" t="s">
         <v>192</v>
-      </c>
-      <c r="F108" s="11" t="s">
-        <v>193</v>
       </c>
       <c r="G108" s="12"/>
       <c r="H108" s="12">
@@ -3776,10 +3783,10 @@
         <v>8</v>
       </c>
       <c r="D109" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E109" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F109" s="11"/>
       <c r="G109" s="12"/>
@@ -3798,10 +3805,10 @@
         <v>8</v>
       </c>
       <c r="D110" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E110" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F110" s="11"/>
       <c r="G110" s="12"/>
@@ -3823,7 +3830,7 @@
         <v>110</v>
       </c>
       <c r="E111" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F111" s="11"/>
       <c r="G111" s="12"/>
@@ -3843,7 +3850,7 @@
       </c>
       <c r="D112" s="6"/>
       <c r="E112" s="13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F112" s="13"/>
       <c r="G112" s="14"/>
@@ -3863,7 +3870,7 @@
         <v>94</v>
       </c>
       <c r="E113" s="13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F113" s="13"/>
       <c r="G113" s="14"/>
@@ -3883,7 +3890,7 @@
         <v>94</v>
       </c>
       <c r="E114" s="13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F114" s="13"/>
       <c r="G114" s="14"/>
@@ -3903,7 +3910,7 @@
         <v>58</v>
       </c>
       <c r="E115" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F115" s="15"/>
       <c r="G115" s="16">
@@ -3922,10 +3929,10 @@
         <v>11</v>
       </c>
       <c r="D116" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E116" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F116" s="11"/>
       <c r="G116" s="12">
@@ -3949,7 +3956,7 @@
         <v>55</v>
       </c>
       <c r="E117" s="23" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F117" s="23"/>
       <c r="G117" s="24">
@@ -3971,7 +3978,7 @@
         <v>55</v>
       </c>
       <c r="E118" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F118" s="11"/>
       <c r="G118" s="12">
@@ -3995,7 +4002,7 @@
         <v>55</v>
       </c>
       <c r="E119" s="11" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F119" s="11"/>
       <c r="G119" s="12">
@@ -4017,10 +4024,10 @@
       </c>
       <c r="D120" s="7"/>
       <c r="E120" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F120" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G120" s="16">
         <v>42192</v>
@@ -4041,10 +4048,10 @@
         <v>55</v>
       </c>
       <c r="E121" s="11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F121" s="11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G121" s="12">
         <v>42192</v>
@@ -4067,7 +4074,7 @@
         <v>55</v>
       </c>
       <c r="E122" s="23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F122" s="23"/>
       <c r="G122" s="24">
@@ -4089,7 +4096,7 @@
         <v>55</v>
       </c>
       <c r="E123" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F123" s="11"/>
       <c r="G123" s="12">
@@ -4113,7 +4120,7 @@
         <v>121</v>
       </c>
       <c r="E124" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F124" s="11"/>
       <c r="G124" s="12">
@@ -4137,7 +4144,7 @@
         <v>121</v>
       </c>
       <c r="E125" s="11" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F125" s="11"/>
       <c r="G125" s="12">
@@ -4159,10 +4166,10 @@
       </c>
       <c r="D126" s="22"/>
       <c r="E126" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="F126" s="23" t="s">
         <v>216</v>
-      </c>
-      <c r="F126" s="23" t="s">
-        <v>217</v>
       </c>
       <c r="G126" s="24">
         <v>42192</v>
@@ -4183,10 +4190,10 @@
         <v>108</v>
       </c>
       <c r="E127" s="23" t="s">
+        <v>246</v>
+      </c>
+      <c r="F127" s="23" t="s">
         <v>247</v>
-      </c>
-      <c r="F127" s="23" t="s">
-        <v>248</v>
       </c>
       <c r="G127" s="24">
         <v>42192</v>
@@ -4205,10 +4212,10 @@
       </c>
       <c r="D128" s="22"/>
       <c r="E128" s="23" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F128" s="23" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="G128" s="24">
         <v>42192</v>
@@ -4229,10 +4236,10 @@
         <v>94</v>
       </c>
       <c r="E129" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="F129" s="11" t="s">
         <v>219</v>
-      </c>
-      <c r="F129" s="11" t="s">
-        <v>220</v>
       </c>
       <c r="G129" s="12">
         <v>42192</v>
@@ -4250,13 +4257,13 @@
         <v>8</v>
       </c>
       <c r="D130" s="22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E130" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="F130" s="23" t="s">
         <v>221</v>
-      </c>
-      <c r="F130" s="23" t="s">
-        <v>222</v>
       </c>
       <c r="G130" s="24">
         <v>42192</v>
@@ -4274,13 +4281,13 @@
         <v>8</v>
       </c>
       <c r="D131" s="22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E131" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="F131" s="23" t="s">
         <v>224</v>
-      </c>
-      <c r="F131" s="23" t="s">
-        <v>225</v>
       </c>
       <c r="G131" s="24">
         <v>42192</v>
@@ -4298,13 +4305,13 @@
         <v>8</v>
       </c>
       <c r="D132" s="22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E132" s="23" t="s">
+        <v>225</v>
+      </c>
+      <c r="F132" s="23" t="s">
         <v>226</v>
-      </c>
-      <c r="F132" s="23" t="s">
-        <v>227</v>
       </c>
       <c r="G132" s="24">
         <v>42192</v>
@@ -4325,7 +4332,7 @@
         <v>121</v>
       </c>
       <c r="E133" s="11" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F133" s="11"/>
       <c r="G133" s="12">
@@ -4349,10 +4356,10 @@
         <v>121</v>
       </c>
       <c r="E134" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F134" s="11" t="s">
         <v>229</v>
-      </c>
-      <c r="F134" s="11" t="s">
-        <v>230</v>
       </c>
       <c r="G134" s="12">
         <v>42193</v>
@@ -4375,7 +4382,7 @@
         <v>121</v>
       </c>
       <c r="E135" s="23" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F135" s="23"/>
       <c r="G135" s="24">
@@ -4397,7 +4404,7 @@
         <v>121</v>
       </c>
       <c r="E136" s="23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F136" s="23"/>
       <c r="G136" s="24">
@@ -4419,10 +4426,10 @@
         <v>121</v>
       </c>
       <c r="E137" s="23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F137" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G137" s="24">
         <v>42193</v>
@@ -4443,7 +4450,7 @@
         <v>121</v>
       </c>
       <c r="E138" s="34" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F138" s="34"/>
       <c r="G138" s="35">
@@ -4462,10 +4469,10 @@
         <v>8</v>
       </c>
       <c r="D139" s="22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E139" s="23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F139" s="23"/>
       <c r="G139" s="24">
@@ -4485,10 +4492,10 @@
       </c>
       <c r="D140" s="25"/>
       <c r="E140" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F140" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G140" s="27">
         <v>42206</v>
@@ -4509,7 +4516,7 @@
         <v>21</v>
       </c>
       <c r="E141" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F141" s="23"/>
       <c r="G141" s="24">
@@ -4531,7 +4538,7 @@
         <v>58</v>
       </c>
       <c r="E142" s="23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F142" s="23"/>
       <c r="G142" s="24">
@@ -4544,14 +4551,14 @@
         <v>142</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C143" s="16" t="s">
         <v>11</v>
       </c>
       <c r="D143" s="7"/>
       <c r="E143" s="15" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F143" s="15"/>
       <c r="G143" s="16">
@@ -4573,10 +4580,10 @@
         <v>94</v>
       </c>
       <c r="E144" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="F144" s="11" t="s">
         <v>245</v>
-      </c>
-      <c r="F144" s="11" t="s">
-        <v>246</v>
       </c>
       <c r="G144" s="12">
         <v>42206</v>
@@ -4599,7 +4606,7 @@
         <v>94</v>
       </c>
       <c r="E145" s="23" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F145" s="23"/>
       <c r="G145" s="24">
@@ -4621,10 +4628,10 @@
         <v>94</v>
       </c>
       <c r="E146" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="F146" s="23" t="s">
         <v>253</v>
-      </c>
-      <c r="F146" s="23" t="s">
-        <v>254</v>
       </c>
       <c r="G146" s="24">
         <v>42214</v>
@@ -4645,10 +4652,10 @@
         <v>25</v>
       </c>
       <c r="E147" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F147" s="11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G147" s="12">
         <v>42214</v>
@@ -4671,7 +4678,7 @@
         <v>25</v>
       </c>
       <c r="E148" s="15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F148" s="15"/>
       <c r="G148" s="16">
@@ -4693,7 +4700,7 @@
         <v>94</v>
       </c>
       <c r="E149" s="23" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F149" s="23"/>
       <c r="G149" s="24">
@@ -4713,10 +4720,10 @@
       </c>
       <c r="D150" s="8"/>
       <c r="E150" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="F150" s="17" t="s">
         <v>265</v>
-      </c>
-      <c r="F150" s="17" t="s">
-        <v>266</v>
       </c>
       <c r="G150" s="18">
         <v>42317</v>
@@ -5579,37 +5586,37 @@
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="10"/>
       <c r="B1" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="22"/>
       <c r="B4" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A5" s="28"/>
       <c r="B5" s="29" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="25"/>
       <c r="B6" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
You can now specify a custom URL for form blocks to be submitted to.
</commit_message>
<xml_diff>
--- a/_SolutionItems/ToDo.xlsx
+++ b/_SolutionItems/ToDo.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="275">
   <si>
     <t>Type</t>
   </si>
@@ -871,6 +871,12 @@
   </si>
   <si>
     <t>Finally solved it! Was indeed a Visual Studio issue. Nop has the same problem.</t>
+  </si>
+  <si>
+    <t>Apply AdminLTE Theme (https://almsaeedstudio.com/) as admin theme for main KoreCMS solution.</t>
+  </si>
+  <si>
+    <t>Will be better than just a plain, ugly theme</t>
   </si>
 </sst>
 </file>
@@ -1455,8 +1461,8 @@
   <dimension ref="A1:H229"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E84" sqref="E84"/>
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F151" sqref="F151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4730,17 +4736,29 @@
       </c>
       <c r="H150" s="18"/>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A151" s="2">
+    <row r="151" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A151" s="22">
         <v>150</v>
       </c>
-      <c r="B151" s="2"/>
-      <c r="C151" s="2"/>
-      <c r="D151" s="2"/>
-      <c r="E151" s="4"/>
-      <c r="F151" s="4"/>
-      <c r="G151" s="3"/>
-      <c r="H151" s="3"/>
+      <c r="B151" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C151" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D151" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="E151" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="F151" s="23" t="s">
+        <v>274</v>
+      </c>
+      <c r="G151" s="24">
+        <v>42402</v>
+      </c>
+      <c r="H151" s="24"/>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152" s="2">

</xml_diff>

<commit_message>
Started work on live chat plugin.
</commit_message>
<xml_diff>
--- a/_SolutionItems/ToDo.xlsx
+++ b/_SolutionItems/ToDo.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="273">
   <si>
     <t>Type</t>
   </si>
@@ -871,12 +871,6 @@
   </si>
   <si>
     <t>Finally solved it! Was indeed a Visual Studio issue. Nop has the same problem.</t>
-  </si>
-  <si>
-    <t>Apply AdminLTE Theme (https://almsaeedstudio.com/) as admin theme for main KoreCMS solution.</t>
-  </si>
-  <si>
-    <t>Will be better than just a plain, ugly theme</t>
   </si>
 </sst>
 </file>
@@ -1458,11 +1452,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H229"/>
+  <dimension ref="A1:H228"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F151" sqref="F151"/>
+      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E152" sqref="E152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4736,33 +4730,21 @@
       </c>
       <c r="H150" s="18"/>
     </row>
-    <row r="151" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A151" s="22">
-        <v>150</v>
-      </c>
-      <c r="B151" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C151" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D151" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="E151" s="23" t="s">
-        <v>273</v>
-      </c>
-      <c r="F151" s="23" t="s">
-        <v>274</v>
-      </c>
-      <c r="G151" s="24">
-        <v>42402</v>
-      </c>
-      <c r="H151" s="24"/>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A151" s="2">
+        <v>151</v>
+      </c>
+      <c r="B151" s="2"/>
+      <c r="C151" s="2"/>
+      <c r="D151" s="2"/>
+      <c r="E151" s="4"/>
+      <c r="F151" s="4"/>
+      <c r="G151" s="3"/>
+      <c r="H151" s="3"/>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A152" s="2">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
@@ -4774,7 +4756,7 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A153" s="2">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
@@ -4786,7 +4768,7 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154" s="2">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
@@ -4798,7 +4780,7 @@
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A155" s="2">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
@@ -4810,7 +4792,7 @@
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A156" s="2">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
@@ -4822,7 +4804,7 @@
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A157" s="2">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
@@ -4834,7 +4816,7 @@
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A158" s="2">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
@@ -4846,7 +4828,7 @@
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A159" s="2">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
@@ -4858,7 +4840,7 @@
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A160" s="2">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
@@ -4870,7 +4852,7 @@
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A161" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B161" s="2"/>
       <c r="C161" s="2"/>
@@ -4882,7 +4864,7 @@
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A162" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
@@ -4894,7 +4876,7 @@
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A163" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
@@ -4906,7 +4888,7 @@
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A164" s="2">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>
@@ -4918,7 +4900,7 @@
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A165" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B165" s="2"/>
       <c r="C165" s="2"/>
@@ -4930,7 +4912,7 @@
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A166" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B166" s="2"/>
       <c r="C166" s="2"/>
@@ -4942,7 +4924,7 @@
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A167" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B167" s="2"/>
       <c r="C167" s="2"/>
@@ -4954,7 +4936,7 @@
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A168" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B168" s="2"/>
       <c r="C168" s="2"/>
@@ -4966,7 +4948,7 @@
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A169" s="2">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
@@ -4978,7 +4960,7 @@
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A170" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B170" s="2"/>
       <c r="C170" s="2"/>
@@ -4989,9 +4971,7 @@
       <c r="H170" s="3"/>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A171" s="2">
-        <v>170</v>
-      </c>
+      <c r="A171" s="2"/>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
       <c r="D171" s="2"/>
@@ -5569,16 +5549,6 @@
       <c r="F228" s="4"/>
       <c r="G228" s="3"/>
       <c r="H228" s="3"/>
-    </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A229" s="2"/>
-      <c r="B229" s="2"/>
-      <c r="C229" s="2"/>
-      <c r="D229" s="2"/>
-      <c r="E229" s="4"/>
-      <c r="F229" s="4"/>
-      <c r="G229" s="3"/>
-      <c r="H229" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Missing content zones are now automatically created - PostgreSQL supported - Bug fixes
</commit_message>
<xml_diff>
--- a/_SolutionItems/ToDo.xlsx
+++ b/_SolutionItems/ToDo.xlsx
@@ -19,6 +19,7 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="277">
   <si>
     <t>Type</t>
   </si>
@@ -871,6 +872,18 @@
   </si>
   <si>
     <t>Finally solved it! Was indeed a Visual Studio issue. Nop has the same problem.</t>
+  </si>
+  <si>
+    <t>Regions: Add coordinates / geo data</t>
+  </si>
+  <si>
+    <t>Errors loading kendo culture file when current culture is NULL</t>
+  </si>
+  <si>
+    <t>For all blocks, change CheckBox to CheckBoxFor</t>
+  </si>
+  <si>
+    <t>They are now automatically created whenever an Html.ContentZone(zoneName) is hit and the specified zone does not exist</t>
   </si>
 </sst>
 </file>
@@ -1265,6 +1278,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1300,6 +1330,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1454,9 +1501,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H228"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G139" sqref="G139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4459,26 +4506,30 @@
       <c r="H138" s="35"/>
     </row>
     <row r="139" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A139" s="22">
+      <c r="A139" s="10">
         <v>138</v>
       </c>
-      <c r="B139" s="22" t="s">
+      <c r="B139" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C139" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D139" s="22" t="s">
+      <c r="C139" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D139" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="E139" s="23" t="s">
+      <c r="E139" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="F139" s="23"/>
-      <c r="G139" s="24">
+      <c r="F139" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="G139" s="12">
         <v>42195</v>
       </c>
-      <c r="H139" s="24"/>
+      <c r="H139" s="12">
+        <v>42455</v>
+      </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A140" s="25">
@@ -4731,40 +4782,68 @@
       <c r="H150" s="18"/>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A151" s="2">
+      <c r="A151" s="22">
         <v>151</v>
       </c>
-      <c r="B151" s="2"/>
-      <c r="C151" s="2"/>
-      <c r="D151" s="2"/>
-      <c r="E151" s="4"/>
-      <c r="F151" s="4"/>
-      <c r="G151" s="3"/>
-      <c r="H151" s="3"/>
+      <c r="B151" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C151" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D151" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="E151" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="F151" s="23"/>
+      <c r="G151" s="24">
+        <v>42455</v>
+      </c>
+      <c r="H151" s="24"/>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A152" s="2">
+      <c r="A152" s="22">
         <v>152</v>
       </c>
-      <c r="B152" s="2"/>
-      <c r="C152" s="2"/>
-      <c r="D152" s="2"/>
-      <c r="E152" s="4"/>
-      <c r="F152" s="4"/>
-      <c r="G152" s="3"/>
-      <c r="H152" s="3"/>
+      <c r="B152" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C152" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D152" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="E152" s="23" t="s">
+        <v>274</v>
+      </c>
+      <c r="F152" s="23"/>
+      <c r="G152" s="24">
+        <v>42455</v>
+      </c>
+      <c r="H152" s="24"/>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A153" s="2">
+      <c r="A153" s="22">
         <v>153</v>
       </c>
-      <c r="B153" s="2"/>
-      <c r="C153" s="2"/>
-      <c r="D153" s="2"/>
-      <c r="E153" s="4"/>
-      <c r="F153" s="4"/>
-      <c r="G153" s="3"/>
-      <c r="H153" s="3"/>
+      <c r="B153" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C153" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D153" s="22"/>
+      <c r="E153" s="23" t="s">
+        <v>275</v>
+      </c>
+      <c r="F153" s="23"/>
+      <c r="G153" s="24">
+        <v>42455</v>
+      </c>
+      <c r="H153" s="24"/>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A154" s="2">

</xml_diff>

<commit_message>
Work on tenants: Settings, Themes and Log
</commit_message>
<xml_diff>
--- a/_SolutionItems/ToDo.xlsx
+++ b/_SolutionItems/ToDo.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Ran\KoreCMS\_SolutionItems\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Ran\KoreCMS_Tenants\_SolutionItems\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
-    <sheet name="Legend" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Legend" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="300">
   <si>
     <t>Type</t>
   </si>
@@ -885,12 +885,81 @@
   <si>
     <t>They are now automatically created whenever an Html.ContentZone(zoneName) is hit and the specified zone does not exist</t>
   </si>
+  <si>
+    <t>Features to modify for tenants:</t>
+  </si>
+  <si>
+    <t>- Indexing?</t>
+  </si>
+  <si>
+    <t>- Logging</t>
+  </si>
+  <si>
+    <t>- Plugins</t>
+  </si>
+  <si>
+    <t>- Settings</t>
+  </si>
+  <si>
+    <t>- Themes</t>
+  </si>
+  <si>
+    <t>- Scheduled Tasks</t>
+  </si>
+  <si>
+    <t>- Regions</t>
+  </si>
+  <si>
+    <t>- Blog</t>
+  </si>
+  <si>
+    <t>- ContentBlocks</t>
+  </si>
+  <si>
+    <t>- Localization</t>
+  </si>
+  <si>
+    <t>- Media</t>
+  </si>
+  <si>
+    <t>- Menus</t>
+  </si>
+  <si>
+    <t>- Messaging</t>
+  </si>
+  <si>
+    <t>- Newsletters</t>
+  </si>
+  <si>
+    <t>- Pages</t>
+  </si>
+  <si>
+    <t>- Sitemap</t>
+  </si>
+  <si>
+    <t>- Caching?</t>
+  </si>
+  <si>
+    <t>Plugins to modify for tenants:</t>
+  </si>
+  <si>
+    <t>- Forums</t>
+  </si>
+  <si>
+    <t>- Watchdog</t>
+  </si>
+  <si>
+    <t>- Live Chat</t>
+  </si>
+  <si>
+    <t>Ready for Test</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -945,6 +1014,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1095,7 +1172,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1152,6 +1229,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="7" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1501,25 +1580,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A136" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G139" sqref="G139"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="59.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="73.44140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="73.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
@@ -1545,7 +1624,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1565,7 +1644,7 @@
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>2</v>
       </c>
@@ -1587,7 +1666,7 @@
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
     </row>
-    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="25">
         <v>3</v>
       </c>
@@ -1611,7 +1690,7 @@
         <v>42237</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -1631,7 +1710,7 @@
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>5</v>
       </c>
@@ -1655,7 +1734,7 @@
         <v>42213</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>6</v>
       </c>
@@ -1679,7 +1758,7 @@
         <v>42345</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -1699,7 +1778,7 @@
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
@@ -1717,7 +1796,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -1739,7 +1818,7 @@
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -1761,7 +1840,7 @@
         <v>42345</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -1783,7 +1862,7 @@
         <v>42207</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -1803,7 +1882,7 @@
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
     </row>
-    <row r="14" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9">
         <v>13</v>
       </c>
@@ -1825,7 +1904,7 @@
       <c r="G14" s="21"/>
       <c r="H14" s="21"/>
     </row>
-    <row r="15" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>14</v>
       </c>
@@ -1847,7 +1926,7 @@
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -1869,7 +1948,7 @@
         <v>42208</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -1893,7 +1972,7 @@
         <v>42213</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -1913,7 +1992,7 @@
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>18</v>
       </c>
@@ -1933,7 +2012,7 @@
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -1955,7 +2034,7 @@
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -1979,7 +2058,7 @@
         <v>42170</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>21</v>
       </c>
@@ -2001,7 +2080,7 @@
       <c r="G22" s="16"/>
       <c r="H22" s="16"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>22</v>
       </c>
@@ -2021,7 +2100,7 @@
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
     </row>
-    <row r="24" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -2043,7 +2122,7 @@
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -2065,7 +2144,7 @@
         <v>42208</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -2087,7 +2166,7 @@
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>26</v>
       </c>
@@ -2107,7 +2186,7 @@
       <c r="G27" s="16"/>
       <c r="H27" s="16"/>
     </row>
-    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>27</v>
       </c>
@@ -2129,7 +2208,7 @@
       <c r="G28" s="18"/>
       <c r="H28" s="18"/>
     </row>
-    <row r="29" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>28</v>
       </c>
@@ -2153,7 +2232,7 @@
         <v>42206</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -2175,7 +2254,7 @@
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
     </row>
-    <row r="31" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>30</v>
       </c>
@@ -2197,7 +2276,7 @@
       <c r="G31" s="18"/>
       <c r="H31" s="18"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>31</v>
       </c>
@@ -2217,7 +2296,7 @@
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>32</v>
       </c>
@@ -2239,7 +2318,7 @@
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="10">
         <v>33</v>
       </c>
@@ -2261,7 +2340,7 @@
         <v>42275</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>34</v>
       </c>
@@ -2281,7 +2360,7 @@
       <c r="G35" s="16"/>
       <c r="H35" s="16"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>35</v>
       </c>
@@ -2301,7 +2380,7 @@
       <c r="G36" s="16"/>
       <c r="H36" s="16"/>
     </row>
-    <row r="37" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="150" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>36</v>
       </c>
@@ -2323,7 +2402,7 @@
       <c r="G37" s="16"/>
       <c r="H37" s="16"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>37</v>
       </c>
@@ -2343,7 +2422,7 @@
       <c r="G38" s="16"/>
       <c r="H38" s="16"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>38</v>
       </c>
@@ -2363,7 +2442,7 @@
       <c r="G39" s="16"/>
       <c r="H39" s="16"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>39</v>
       </c>
@@ -2385,7 +2464,7 @@
       <c r="G40" s="16"/>
       <c r="H40" s="16"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>40</v>
       </c>
@@ -2405,7 +2484,7 @@
       <c r="G41" s="14"/>
       <c r="H41" s="14"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>41</v>
       </c>
@@ -2425,7 +2504,7 @@
       <c r="G42" s="14"/>
       <c r="H42" s="14"/>
     </row>
-    <row r="43" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>42</v>
       </c>
@@ -2447,7 +2526,7 @@
       <c r="G43" s="16"/>
       <c r="H43" s="16"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>43</v>
       </c>
@@ -2469,7 +2548,7 @@
       <c r="G44" s="14"/>
       <c r="H44" s="14"/>
     </row>
-    <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
         <v>44</v>
       </c>
@@ -2489,7 +2568,7 @@
       <c r="G45" s="14"/>
       <c r="H45" s="14"/>
     </row>
-    <row r="46" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="30">
         <v>45</v>
       </c>
@@ -2511,7 +2590,7 @@
         <v>42400</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="9">
         <v>46</v>
       </c>
@@ -2531,7 +2610,7 @@
       <c r="G47" s="21"/>
       <c r="H47" s="21"/>
     </row>
-    <row r="48" spans="1:8" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="9">
         <v>47</v>
       </c>
@@ -2551,7 +2630,7 @@
       <c r="G48" s="21"/>
       <c r="H48" s="21"/>
     </row>
-    <row r="49" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A49" s="10">
         <v>48</v>
       </c>
@@ -2575,7 +2654,7 @@
         <v>42214</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>49</v>
       </c>
@@ -2595,7 +2674,7 @@
       <c r="G50" s="14"/>
       <c r="H50" s="14"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="6">
         <v>50</v>
       </c>
@@ -2617,7 +2696,7 @@
       <c r="G51" s="14"/>
       <c r="H51" s="14"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="10">
         <v>51</v>
       </c>
@@ -2637,7 +2716,7 @@
         <v>42239</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="19">
         <v>52</v>
       </c>
@@ -2657,7 +2736,7 @@
       <c r="G53" s="14"/>
       <c r="H53" s="14"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="6">
         <v>53</v>
       </c>
@@ -2675,7 +2754,7 @@
       <c r="G54" s="14"/>
       <c r="H54" s="14"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="6">
         <v>54</v>
       </c>
@@ -2695,7 +2774,7 @@
       <c r="G55" s="14"/>
       <c r="H55" s="14"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
         <v>55</v>
       </c>
@@ -2715,7 +2794,7 @@
       <c r="G56" s="14"/>
       <c r="H56" s="14"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="6">
         <v>56</v>
       </c>
@@ -2735,7 +2814,7 @@
       <c r="G57" s="14"/>
       <c r="H57" s="14"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="6">
         <v>57</v>
       </c>
@@ -2755,7 +2834,7 @@
       <c r="G58" s="14"/>
       <c r="H58" s="14"/>
     </row>
-    <row r="59" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="6">
         <v>58</v>
       </c>
@@ -2773,7 +2852,7 @@
       <c r="G59" s="14"/>
       <c r="H59" s="14"/>
     </row>
-    <row r="60" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="9">
         <v>59</v>
       </c>
@@ -2793,7 +2872,7 @@
       <c r="G60" s="21"/>
       <c r="H60" s="21"/>
     </row>
-    <row r="61" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A61" s="6">
         <v>60</v>
       </c>
@@ -2813,7 +2892,7 @@
       <c r="G61" s="14"/>
       <c r="H61" s="14"/>
     </row>
-    <row r="62" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
         <v>61</v>
       </c>
@@ -2835,7 +2914,7 @@
       <c r="G62" s="16"/>
       <c r="H62" s="16"/>
     </row>
-    <row r="63" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="10">
         <v>62</v>
       </c>
@@ -2857,7 +2936,7 @@
         <v>42238</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="6">
         <v>63</v>
       </c>
@@ -2877,7 +2956,7 @@
       <c r="G64" s="14"/>
       <c r="H64" s="14"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="6">
         <v>64</v>
       </c>
@@ -2897,7 +2976,7 @@
       <c r="G65" s="14"/>
       <c r="H65" s="14"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
         <v>65</v>
       </c>
@@ -2919,7 +2998,7 @@
       <c r="G66" s="14"/>
       <c r="H66" s="14"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="6">
         <v>66</v>
       </c>
@@ -2941,7 +3020,7 @@
       <c r="G67" s="14"/>
       <c r="H67" s="14"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="8">
         <v>67</v>
       </c>
@@ -2963,7 +3042,7 @@
       <c r="G68" s="18"/>
       <c r="H68" s="18"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="6">
         <v>68</v>
       </c>
@@ -2983,7 +3062,7 @@
       <c r="G69" s="14"/>
       <c r="H69" s="14"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="10">
         <v>69</v>
       </c>
@@ -3003,7 +3082,7 @@
       <c r="G70" s="12"/>
       <c r="H70" s="12"/>
     </row>
-    <row r="71" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="6">
         <v>70</v>
       </c>
@@ -3023,7 +3102,7 @@
       <c r="G71" s="14"/>
       <c r="H71" s="14"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="6">
         <v>71</v>
       </c>
@@ -3045,7 +3124,7 @@
       <c r="G72" s="14"/>
       <c r="H72" s="14"/>
     </row>
-    <row r="73" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A73" s="6">
         <v>72</v>
       </c>
@@ -3067,7 +3146,7 @@
       <c r="G73" s="14"/>
       <c r="H73" s="14"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="19">
         <v>73</v>
       </c>
@@ -3087,7 +3166,7 @@
       <c r="G74" s="14"/>
       <c r="H74" s="14"/>
     </row>
-    <row r="75" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="6">
         <v>74</v>
       </c>
@@ -3107,7 +3186,7 @@
       <c r="G75" s="14"/>
       <c r="H75" s="14"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="8">
         <v>75</v>
       </c>
@@ -3129,7 +3208,7 @@
       <c r="G76" s="18"/>
       <c r="H76" s="18"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="6">
         <v>76</v>
       </c>
@@ -3149,7 +3228,7 @@
       <c r="G77" s="14"/>
       <c r="H77" s="14"/>
     </row>
-    <row r="78" spans="1:8" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="10">
         <v>77</v>
       </c>
@@ -3173,7 +3252,7 @@
         <v>42238</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="9">
         <v>78</v>
       </c>
@@ -3191,7 +3270,7 @@
       <c r="G79" s="21"/>
       <c r="H79" s="21"/>
     </row>
-    <row r="80" spans="1:8" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A80" s="6">
         <v>79</v>
       </c>
@@ -3213,7 +3292,7 @@
       <c r="G80" s="14"/>
       <c r="H80" s="14"/>
     </row>
-    <row r="81" spans="1:8" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" ht="270" x14ac:dyDescent="0.25">
       <c r="A81" s="6">
         <v>80</v>
       </c>
@@ -3233,7 +3312,7 @@
       <c r="G81" s="14"/>
       <c r="H81" s="14"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="6">
         <v>81</v>
       </c>
@@ -3253,7 +3332,7 @@
       <c r="G82" s="14"/>
       <c r="H82" s="14"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="6">
         <v>82</v>
       </c>
@@ -3273,7 +3352,7 @@
       <c r="G83" s="14"/>
       <c r="H83" s="14"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="6">
         <v>83</v>
       </c>
@@ -3295,7 +3374,7 @@
       <c r="G84" s="14"/>
       <c r="H84" s="14"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="10">
         <v>84</v>
       </c>
@@ -3317,7 +3396,7 @@
         <v>42402</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="6">
         <v>85</v>
       </c>
@@ -3339,7 +3418,7 @@
       <c r="G86" s="14"/>
       <c r="H86" s="14"/>
     </row>
-    <row r="87" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="30">
         <v>86</v>
       </c>
@@ -3361,7 +3440,7 @@
         <v>42238</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:8" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="9">
         <v>87</v>
       </c>
@@ -3383,7 +3462,7 @@
       <c r="G88" s="21"/>
       <c r="H88" s="21"/>
     </row>
-    <row r="89" spans="1:8" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:8" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="9">
         <v>88</v>
       </c>
@@ -3405,7 +3484,7 @@
       <c r="G89" s="21"/>
       <c r="H89" s="21"/>
     </row>
-    <row r="90" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A90" s="25">
         <v>89</v>
       </c>
@@ -3427,7 +3506,7 @@
       <c r="G90" s="27"/>
       <c r="H90" s="27"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="6">
         <v>90</v>
       </c>
@@ -3445,7 +3524,7 @@
       <c r="G91" s="14"/>
       <c r="H91" s="14"/>
     </row>
-    <row r="92" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="25">
         <v>91</v>
       </c>
@@ -3467,7 +3546,7 @@
       <c r="G92" s="27"/>
       <c r="H92" s="27"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="6">
         <v>92</v>
       </c>
@@ -3489,7 +3568,7 @@
       <c r="G93" s="14"/>
       <c r="H93" s="14"/>
     </row>
-    <row r="94" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="10">
         <v>93</v>
       </c>
@@ -3513,7 +3592,7 @@
         <v>42389</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="9">
         <v>94</v>
       </c>
@@ -3533,7 +3612,7 @@
       <c r="G95" s="21"/>
       <c r="H95" s="21"/>
     </row>
-    <row r="96" spans="1:8" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:8" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="9">
         <v>95</v>
       </c>
@@ -3555,7 +3634,7 @@
       <c r="G96" s="21"/>
       <c r="H96" s="21"/>
     </row>
-    <row r="97" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A97" s="25">
         <v>96</v>
       </c>
@@ -3577,7 +3656,7 @@
       <c r="G97" s="27"/>
       <c r="H97" s="27"/>
     </row>
-    <row r="98" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A98" s="6">
         <v>97</v>
       </c>
@@ -3599,7 +3678,7 @@
       <c r="G98" s="14"/>
       <c r="H98" s="14"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="7">
         <v>98</v>
       </c>
@@ -3619,7 +3698,7 @@
       <c r="G99" s="16"/>
       <c r="H99" s="16"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="6">
         <v>99</v>
       </c>
@@ -3639,7 +3718,7 @@
       <c r="G100" s="14"/>
       <c r="H100" s="14"/>
     </row>
-    <row r="101" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A101" s="6">
         <v>100</v>
       </c>
@@ -3661,7 +3740,7 @@
       <c r="G101" s="14"/>
       <c r="H101" s="14"/>
     </row>
-    <row r="102" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A102" s="10">
         <v>101</v>
       </c>
@@ -3685,7 +3764,7 @@
         <v>42213</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="9">
         <v>102</v>
       </c>
@@ -3707,7 +3786,7 @@
       <c r="G103" s="21"/>
       <c r="H103" s="21"/>
     </row>
-    <row r="104" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A104" s="6">
         <v>103</v>
       </c>
@@ -3729,7 +3808,7 @@
       <c r="G104" s="14"/>
       <c r="H104" s="14"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="6">
         <v>104</v>
       </c>
@@ -3751,7 +3830,7 @@
       <c r="G105" s="14"/>
       <c r="H105" s="14"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="10">
         <v>105</v>
       </c>
@@ -3773,7 +3852,7 @@
         <v>42188</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A107" s="10">
         <v>106</v>
       </c>
@@ -3795,7 +3874,7 @@
         <v>42214</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="10">
         <v>107</v>
       </c>
@@ -3819,7 +3898,7 @@
         <v>42188</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="10">
         <v>108</v>
       </c>
@@ -3841,7 +3920,7 @@
         <v>42188</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="10">
         <v>109</v>
       </c>
@@ -3863,7 +3942,7 @@
         <v>42188</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A111" s="10">
         <v>110</v>
       </c>
@@ -3885,7 +3964,7 @@
         <v>42188</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="6">
         <v>111</v>
       </c>
@@ -3903,7 +3982,7 @@
       <c r="G112" s="14"/>
       <c r="H112" s="14"/>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="6">
         <v>112</v>
       </c>
@@ -3923,7 +4002,7 @@
       <c r="G113" s="14"/>
       <c r="H113" s="14"/>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="6">
         <v>113</v>
       </c>
@@ -3943,7 +4022,7 @@
       <c r="G114" s="14"/>
       <c r="H114" s="14"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="7">
         <v>114</v>
       </c>
@@ -3965,7 +4044,7 @@
       </c>
       <c r="H115" s="16"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="10">
         <v>115</v>
       </c>
@@ -3989,7 +4068,7 @@
         <v>42188</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="22">
         <v>116</v>
       </c>
@@ -4011,7 +4090,7 @@
       </c>
       <c r="H117" s="24"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="10">
         <v>117</v>
       </c>
@@ -4035,7 +4114,7 @@
         <v>42206</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="10">
         <v>118</v>
       </c>
@@ -4059,7 +4138,7 @@
         <v>42195</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="7">
         <v>119</v>
       </c>
@@ -4081,7 +4160,7 @@
       </c>
       <c r="H120" s="16"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="10">
         <v>120</v>
       </c>
@@ -4107,7 +4186,7 @@
         <v>42195</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="22">
         <v>121</v>
       </c>
@@ -4129,7 +4208,7 @@
       </c>
       <c r="H122" s="24"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="10">
         <v>122</v>
       </c>
@@ -4153,7 +4232,7 @@
         <v>42195</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="10">
         <v>123</v>
       </c>
@@ -4177,7 +4256,7 @@
         <v>42194</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="10">
         <v>124</v>
       </c>
@@ -4201,7 +4280,7 @@
         <v>42194</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="22">
         <v>125</v>
       </c>
@@ -4223,7 +4302,7 @@
       </c>
       <c r="H126" s="24"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="22">
         <v>126</v>
       </c>
@@ -4247,7 +4326,7 @@
       </c>
       <c r="H127" s="24"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="22">
         <v>127</v>
       </c>
@@ -4269,7 +4348,7 @@
       </c>
       <c r="H128" s="24"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A129" s="10">
         <v>128</v>
       </c>
@@ -4293,7 +4372,7 @@
       </c>
       <c r="H129" s="12"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="22">
         <v>129</v>
       </c>
@@ -4317,7 +4396,7 @@
       </c>
       <c r="H130" s="24"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="22">
         <v>130</v>
       </c>
@@ -4341,7 +4420,7 @@
       </c>
       <c r="H131" s="24"/>
     </row>
-    <row r="132" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A132" s="22">
         <v>131</v>
       </c>
@@ -4365,7 +4444,7 @@
       </c>
       <c r="H132" s="24"/>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="10">
         <v>132</v>
       </c>
@@ -4389,7 +4468,7 @@
         <v>42194</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="10">
         <v>133</v>
       </c>
@@ -4415,7 +4494,7 @@
         <v>42195</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="22">
         <v>134</v>
       </c>
@@ -4437,7 +4516,7 @@
       </c>
       <c r="H135" s="24"/>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="22">
         <v>135</v>
       </c>
@@ -4459,7 +4538,7 @@
       </c>
       <c r="H136" s="24"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="22">
         <v>136</v>
       </c>
@@ -4483,7 +4562,7 @@
       </c>
       <c r="H137" s="24"/>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="33">
         <v>137</v>
       </c>
@@ -4505,7 +4584,7 @@
       </c>
       <c r="H138" s="35"/>
     </row>
-    <row r="139" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="10">
         <v>138</v>
       </c>
@@ -4531,7 +4610,7 @@
         <v>42455</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="25">
         <v>139</v>
       </c>
@@ -4553,7 +4632,7 @@
       </c>
       <c r="H140" s="27"/>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="22">
         <v>140</v>
       </c>
@@ -4575,7 +4654,7 @@
       </c>
       <c r="H141" s="24"/>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="22">
         <v>141</v>
       </c>
@@ -4597,7 +4676,7 @@
       </c>
       <c r="H142" s="24"/>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="7">
         <v>142</v>
       </c>
@@ -4617,7 +4696,7 @@
       </c>
       <c r="H143" s="16"/>
     </row>
-    <row r="144" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A144" s="10">
         <v>143</v>
       </c>
@@ -4643,7 +4722,7 @@
         <v>42238</v>
       </c>
     </row>
-    <row r="145" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A145" s="22">
         <v>144</v>
       </c>
@@ -4665,7 +4744,7 @@
       </c>
       <c r="H145" s="24"/>
     </row>
-    <row r="146" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A146" s="22">
         <v>145</v>
       </c>
@@ -4689,7 +4768,7 @@
       </c>
       <c r="H146" s="24"/>
     </row>
-    <row r="147" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A147" s="10">
         <v>146</v>
       </c>
@@ -4715,7 +4794,7 @@
         <v>42353</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="7">
         <v>147</v>
       </c>
@@ -4737,7 +4816,7 @@
       </c>
       <c r="H148" s="16"/>
     </row>
-    <row r="149" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A149" s="22">
         <v>148</v>
       </c>
@@ -4759,7 +4838,7 @@
       </c>
       <c r="H149" s="24"/>
     </row>
-    <row r="150" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A150" s="8">
         <v>149</v>
       </c>
@@ -4781,7 +4860,7 @@
       </c>
       <c r="H150" s="18"/>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="22">
         <v>151</v>
       </c>
@@ -4803,7 +4882,7 @@
       </c>
       <c r="H151" s="24"/>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="22">
         <v>152</v>
       </c>
@@ -4825,7 +4904,7 @@
       </c>
       <c r="H152" s="24"/>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="22">
         <v>153</v>
       </c>
@@ -4845,7 +4924,7 @@
       </c>
       <c r="H153" s="24"/>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>154</v>
       </c>
@@ -4857,7 +4936,7 @@
       <c r="G154" s="3"/>
       <c r="H154" s="3"/>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>155</v>
       </c>
@@ -4869,7 +4948,7 @@
       <c r="G155" s="3"/>
       <c r="H155" s="3"/>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>156</v>
       </c>
@@ -4881,7 +4960,7 @@
       <c r="G156" s="3"/>
       <c r="H156" s="3"/>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>157</v>
       </c>
@@ -4893,7 +4972,7 @@
       <c r="G157" s="3"/>
       <c r="H157" s="3"/>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>158</v>
       </c>
@@ -4905,7 +4984,7 @@
       <c r="G158" s="3"/>
       <c r="H158" s="3"/>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>159</v>
       </c>
@@ -4917,7 +4996,7 @@
       <c r="G159" s="3"/>
       <c r="H159" s="3"/>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>160</v>
       </c>
@@ -4929,7 +5008,7 @@
       <c r="G160" s="3"/>
       <c r="H160" s="3"/>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>161</v>
       </c>
@@ -4941,7 +5020,7 @@
       <c r="G161" s="3"/>
       <c r="H161" s="3"/>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>162</v>
       </c>
@@ -4953,7 +5032,7 @@
       <c r="G162" s="3"/>
       <c r="H162" s="3"/>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>163</v>
       </c>
@@ -4965,7 +5044,7 @@
       <c r="G163" s="3"/>
       <c r="H163" s="3"/>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <v>164</v>
       </c>
@@ -4977,7 +5056,7 @@
       <c r="G164" s="3"/>
       <c r="H164" s="3"/>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>165</v>
       </c>
@@ -4989,7 +5068,7 @@
       <c r="G165" s="3"/>
       <c r="H165" s="3"/>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>166</v>
       </c>
@@ -5001,7 +5080,7 @@
       <c r="G166" s="3"/>
       <c r="H166" s="3"/>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>167</v>
       </c>
@@ -5013,7 +5092,7 @@
       <c r="G167" s="3"/>
       <c r="H167" s="3"/>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
         <v>168</v>
       </c>
@@ -5025,7 +5104,7 @@
       <c r="G168" s="3"/>
       <c r="H168" s="3"/>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
         <v>169</v>
       </c>
@@ -5037,7 +5116,7 @@
       <c r="G169" s="3"/>
       <c r="H169" s="3"/>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
         <v>170</v>
       </c>
@@ -5049,7 +5128,7 @@
       <c r="G170" s="3"/>
       <c r="H170" s="3"/>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="2"/>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
@@ -5059,7 +5138,7 @@
       <c r="G171" s="3"/>
       <c r="H171" s="3"/>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="2"/>
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
@@ -5069,7 +5148,7 @@
       <c r="G172" s="3"/>
       <c r="H172" s="3"/>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="2"/>
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
@@ -5079,7 +5158,7 @@
       <c r="G173" s="3"/>
       <c r="H173" s="3"/>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="2"/>
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
@@ -5089,7 +5168,7 @@
       <c r="G174" s="3"/>
       <c r="H174" s="3"/>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="2"/>
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
@@ -5099,7 +5178,7 @@
       <c r="G175" s="3"/>
       <c r="H175" s="3"/>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="2"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
@@ -5109,7 +5188,7 @@
       <c r="G176" s="3"/>
       <c r="H176" s="3"/>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="2"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
@@ -5119,7 +5198,7 @@
       <c r="G177" s="3"/>
       <c r="H177" s="3"/>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="2"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
@@ -5129,7 +5208,7 @@
       <c r="G178" s="3"/>
       <c r="H178" s="3"/>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="2"/>
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
@@ -5139,7 +5218,7 @@
       <c r="G179" s="3"/>
       <c r="H179" s="3"/>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="2"/>
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
@@ -5149,7 +5228,7 @@
       <c r="G180" s="3"/>
       <c r="H180" s="3"/>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="2"/>
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
@@ -5159,7 +5238,7 @@
       <c r="G181" s="3"/>
       <c r="H181" s="3"/>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="2"/>
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
@@ -5169,7 +5248,7 @@
       <c r="G182" s="3"/>
       <c r="H182" s="3"/>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="2"/>
       <c r="B183" s="2"/>
       <c r="C183" s="2"/>
@@ -5179,7 +5258,7 @@
       <c r="G183" s="3"/>
       <c r="H183" s="3"/>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="2"/>
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
@@ -5189,7 +5268,7 @@
       <c r="G184" s="3"/>
       <c r="H184" s="3"/>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="2"/>
       <c r="B185" s="2"/>
       <c r="C185" s="2"/>
@@ -5199,7 +5278,7 @@
       <c r="G185" s="3"/>
       <c r="H185" s="3"/>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="2"/>
       <c r="B186" s="2"/>
       <c r="C186" s="2"/>
@@ -5209,7 +5288,7 @@
       <c r="G186" s="3"/>
       <c r="H186" s="3"/>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="2"/>
       <c r="B187" s="2"/>
       <c r="C187" s="2"/>
@@ -5219,7 +5298,7 @@
       <c r="G187" s="3"/>
       <c r="H187" s="3"/>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="2"/>
       <c r="B188" s="2"/>
       <c r="C188" s="2"/>
@@ -5229,7 +5308,7 @@
       <c r="G188" s="3"/>
       <c r="H188" s="3"/>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="2"/>
       <c r="B189" s="2"/>
       <c r="C189" s="2"/>
@@ -5239,7 +5318,7 @@
       <c r="G189" s="3"/>
       <c r="H189" s="3"/>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" s="2"/>
       <c r="B190" s="2"/>
       <c r="C190" s="2"/>
@@ -5249,7 +5328,7 @@
       <c r="G190" s="3"/>
       <c r="H190" s="3"/>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="2"/>
       <c r="B191" s="2"/>
       <c r="C191" s="2"/>
@@ -5259,7 +5338,7 @@
       <c r="G191" s="3"/>
       <c r="H191" s="3"/>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="2"/>
       <c r="B192" s="2"/>
       <c r="C192" s="2"/>
@@ -5269,7 +5348,7 @@
       <c r="G192" s="3"/>
       <c r="H192" s="3"/>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" s="2"/>
       <c r="B193" s="2"/>
       <c r="C193" s="2"/>
@@ -5279,7 +5358,7 @@
       <c r="G193" s="3"/>
       <c r="H193" s="3"/>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" s="2"/>
       <c r="B194" s="2"/>
       <c r="C194" s="2"/>
@@ -5289,7 +5368,7 @@
       <c r="G194" s="3"/>
       <c r="H194" s="3"/>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" s="2"/>
       <c r="B195" s="2"/>
       <c r="C195" s="2"/>
@@ -5299,7 +5378,7 @@
       <c r="G195" s="3"/>
       <c r="H195" s="3"/>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" s="2"/>
       <c r="B196" s="2"/>
       <c r="C196" s="2"/>
@@ -5309,7 +5388,7 @@
       <c r="G196" s="3"/>
       <c r="H196" s="3"/>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" s="2"/>
       <c r="B197" s="2"/>
       <c r="C197" s="2"/>
@@ -5319,7 +5398,7 @@
       <c r="G197" s="3"/>
       <c r="H197" s="3"/>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" s="2"/>
       <c r="B198" s="2"/>
       <c r="C198" s="2"/>
@@ -5329,7 +5408,7 @@
       <c r="G198" s="3"/>
       <c r="H198" s="3"/>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" s="2"/>
       <c r="B199" s="2"/>
       <c r="C199" s="2"/>
@@ -5339,7 +5418,7 @@
       <c r="G199" s="3"/>
       <c r="H199" s="3"/>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" s="2"/>
       <c r="B200" s="2"/>
       <c r="C200" s="2"/>
@@ -5349,7 +5428,7 @@
       <c r="G200" s="3"/>
       <c r="H200" s="3"/>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" s="2"/>
       <c r="B201" s="2"/>
       <c r="C201" s="2"/>
@@ -5359,7 +5438,7 @@
       <c r="G201" s="3"/>
       <c r="H201" s="3"/>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" s="2"/>
       <c r="B202" s="2"/>
       <c r="C202" s="2"/>
@@ -5369,7 +5448,7 @@
       <c r="G202" s="3"/>
       <c r="H202" s="3"/>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" s="2"/>
       <c r="B203" s="2"/>
       <c r="C203" s="2"/>
@@ -5379,7 +5458,7 @@
       <c r="G203" s="3"/>
       <c r="H203" s="3"/>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" s="2"/>
       <c r="B204" s="2"/>
       <c r="C204" s="2"/>
@@ -5389,7 +5468,7 @@
       <c r="G204" s="3"/>
       <c r="H204" s="3"/>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" s="2"/>
       <c r="B205" s="2"/>
       <c r="C205" s="2"/>
@@ -5399,7 +5478,7 @@
       <c r="G205" s="3"/>
       <c r="H205" s="3"/>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" s="2"/>
       <c r="B206" s="2"/>
       <c r="C206" s="2"/>
@@ -5409,7 +5488,7 @@
       <c r="G206" s="3"/>
       <c r="H206" s="3"/>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="2"/>
       <c r="B207" s="2"/>
       <c r="C207" s="2"/>
@@ -5419,7 +5498,7 @@
       <c r="G207" s="3"/>
       <c r="H207" s="3"/>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" s="2"/>
       <c r="B208" s="2"/>
       <c r="C208" s="2"/>
@@ -5429,7 +5508,7 @@
       <c r="G208" s="3"/>
       <c r="H208" s="3"/>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" s="2"/>
       <c r="B209" s="2"/>
       <c r="C209" s="2"/>
@@ -5439,7 +5518,7 @@
       <c r="G209" s="3"/>
       <c r="H209" s="3"/>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" s="2"/>
       <c r="B210" s="2"/>
       <c r="C210" s="2"/>
@@ -5449,7 +5528,7 @@
       <c r="G210" s="3"/>
       <c r="H210" s="3"/>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" s="2"/>
       <c r="B211" s="2"/>
       <c r="C211" s="2"/>
@@ -5459,7 +5538,7 @@
       <c r="G211" s="3"/>
       <c r="H211" s="3"/>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" s="2"/>
       <c r="B212" s="2"/>
       <c r="C212" s="2"/>
@@ -5469,7 +5548,7 @@
       <c r="G212" s="3"/>
       <c r="H212" s="3"/>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" s="2"/>
       <c r="B213" s="2"/>
       <c r="C213" s="2"/>
@@ -5479,7 +5558,7 @@
       <c r="G213" s="3"/>
       <c r="H213" s="3"/>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" s="2"/>
       <c r="B214" s="2"/>
       <c r="C214" s="2"/>
@@ -5489,7 +5568,7 @@
       <c r="G214" s="3"/>
       <c r="H214" s="3"/>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" s="2"/>
       <c r="B215" s="2"/>
       <c r="C215" s="2"/>
@@ -5499,7 +5578,7 @@
       <c r="G215" s="3"/>
       <c r="H215" s="3"/>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" s="2"/>
       <c r="B216" s="2"/>
       <c r="C216" s="2"/>
@@ -5509,7 +5588,7 @@
       <c r="G216" s="3"/>
       <c r="H216" s="3"/>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217" s="2"/>
       <c r="B217" s="2"/>
       <c r="C217" s="2"/>
@@ -5519,7 +5598,7 @@
       <c r="G217" s="3"/>
       <c r="H217" s="3"/>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" s="2"/>
       <c r="B218" s="2"/>
       <c r="C218" s="2"/>
@@ -5529,7 +5608,7 @@
       <c r="G218" s="3"/>
       <c r="H218" s="3"/>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" s="2"/>
       <c r="B219" s="2"/>
       <c r="C219" s="2"/>
@@ -5539,7 +5618,7 @@
       <c r="G219" s="3"/>
       <c r="H219" s="3"/>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A220" s="2"/>
       <c r="B220" s="2"/>
       <c r="C220" s="2"/>
@@ -5549,7 +5628,7 @@
       <c r="G220" s="3"/>
       <c r="H220" s="3"/>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A221" s="2"/>
       <c r="B221" s="2"/>
       <c r="C221" s="2"/>
@@ -5559,7 +5638,7 @@
       <c r="G221" s="3"/>
       <c r="H221" s="3"/>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A222" s="2"/>
       <c r="B222" s="2"/>
       <c r="C222" s="2"/>
@@ -5569,7 +5648,7 @@
       <c r="G222" s="3"/>
       <c r="H222" s="3"/>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A223" s="2"/>
       <c r="B223" s="2"/>
       <c r="C223" s="2"/>
@@ -5579,7 +5658,7 @@
       <c r="G223" s="3"/>
       <c r="H223" s="3"/>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A224" s="2"/>
       <c r="B224" s="2"/>
       <c r="C224" s="2"/>
@@ -5589,7 +5668,7 @@
       <c r="G224" s="3"/>
       <c r="H224" s="3"/>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A225" s="2"/>
       <c r="B225" s="2"/>
       <c r="C225" s="2"/>
@@ -5599,7 +5678,7 @@
       <c r="G225" s="3"/>
       <c r="H225" s="3"/>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A226" s="2"/>
       <c r="B226" s="2"/>
       <c r="C226" s="2"/>
@@ -5609,7 +5688,7 @@
       <c r="G226" s="3"/>
       <c r="H226" s="3"/>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A227" s="2"/>
       <c r="B227" s="2"/>
       <c r="C227" s="2"/>
@@ -5619,7 +5698,7 @@
       <c r="G227" s="3"/>
       <c r="H227" s="3"/>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A228" s="2"/>
       <c r="B228" s="2"/>
       <c r="C228" s="2"/>
@@ -5637,50 +5716,189 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
+        <v>281</v>
+      </c>
+      <c r="B2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
+        <v>282</v>
+      </c>
+      <c r="B3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="36" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="36" t="s">
+        <v>279</v>
+      </c>
+      <c r="B5" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="36" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="36" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="36" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="36" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="36" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="36" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="36" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="36" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="36" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="36" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="36" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="36" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="36" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="37" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="36" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="36" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="36" t="s">
+        <v>298</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="22"/>
       <c r="B4" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="28"/>
       <c r="B5" s="29" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="25"/>
       <c r="B6" s="2" t="s">
         <v>258</v>

</xml_diff>

<commit_message>
Adding tenants code for regions, blog, menus, messaging, newsletters and sitemap. Still needs testing...
</commit_message>
<xml_diff>
--- a/_SolutionItems/ToDo.xlsx
+++ b/_SolutionItems/ToDo.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="304">
   <si>
     <t>Type</t>
   </si>
@@ -962,6 +962,9 @@
   </si>
   <si>
     <t>Maybe not needed</t>
+  </si>
+  <si>
+    <t>Ajax Blog Content not done. Need to look at for future, but not important for now.</t>
   </si>
 </sst>
 </file>
@@ -5744,7 +5747,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5817,11 +5820,20 @@
       <c r="A8" s="36" t="s">
         <v>283</v>
       </c>
+      <c r="B8" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="36" t="s">
         <v>284</v>
       </c>
+      <c r="B9" t="s">
+        <v>298</v>
+      </c>
+      <c r="C9" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="36" t="s">
@@ -5853,16 +5865,25 @@
       <c r="A13" s="36" t="s">
         <v>288</v>
       </c>
+      <c r="B13" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="36" t="s">
         <v>289</v>
       </c>
+      <c r="B14" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="36" t="s">
         <v>290</v>
       </c>
+      <c r="B15" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="40" t="s">
@@ -5873,32 +5894,35 @@
       </c>
       <c r="C16" s="41"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="36" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="36" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="37" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="36" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="36" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="36" t="s">
         <v>297</v>
       </c>

</xml_diff>